<commit_message>
Modification to draw from 2 databases - partially complete, prior to handing over to Marcus
</commit_message>
<xml_diff>
--- a/create-data/create_reference_data/source/measure_types.xlsx
+++ b/create-data/create_reference_data/source/measure_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\tariff\create-data\create_reference_data\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt.admin/projects/tariffs/create-data/create_reference_data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C784332-2BD3-400F-97DE-CC1385C3917B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621E2E69-3E62-B042-8252-DC2FCD265EBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="9555" activeTab="1" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24840" windowHeight="16520" activeTab="1" xr2:uid="{B724F9FD-527C-4A95-969C-B8CCC70DC96A}"/>
   </bookViews>
   <sheets>
     <sheet name="Updated" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -291,9 +291,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -640,130 +637,130 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="75.140625" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="19.83203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="75.1640625" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
         <v>105</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
         <v>123</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
         <v>145</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
         <v>146</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
         <v>552</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
         <v>553</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
         <v>554</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
         <v>555</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
         <v>561</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
         <v>562</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
         <v>564</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
         <v>565</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
         <v>566</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
         <v>570</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -779,55 +776,55 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="24" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="4"/>
-    <col min="8" max="8" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" style="4"/>
+    <col min="8" max="8" width="30.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>130</v>
       </c>
@@ -835,7 +832,7 @@
         <v>54</v>
       </c>
       <c r="C2" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -859,7 +856,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>131</v>
       </c>
@@ -867,7 +864,7 @@
         <v>53</v>
       </c>
       <c r="C3" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -891,7 +888,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>132</v>
       </c>
@@ -899,7 +896,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -923,7 +920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>133</v>
       </c>
@@ -931,7 +928,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -955,7 +952,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>134</v>
       </c>
@@ -963,7 +960,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -987,7 +984,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>350</v>
       </c>
@@ -995,7 +992,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1019,7 +1016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>351</v>
       </c>
@@ -1027,7 +1024,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -1051,7 +1048,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>352</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -1083,7 +1080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>353</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1115,7 +1112,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>354</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1147,7 +1144,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>355</v>
       </c>
@@ -1155,7 +1152,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -1179,39 +1176,39 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>356</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="7">
-        <v>43554</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="C13" s="5">
+        <v>43769</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
         <v>5</v>
       </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8">
-        <v>2</v>
-      </c>
-      <c r="I13" s="8">
-        <v>10</v>
-      </c>
-      <c r="J13" s="8" t="s">
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>10</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>357</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1243,7 +1240,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>358</v>
       </c>
@@ -1251,7 +1248,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -1275,7 +1272,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>359</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D16" s="4">
         <v>0</v>
@@ -1307,7 +1304,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>360</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D17" s="4">
         <v>0</v>
@@ -1339,7 +1336,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>361</v>
       </c>
@@ -1347,7 +1344,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1371,7 +1368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>362</v>
       </c>
@@ -1379,7 +1376,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -1403,7 +1400,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>363</v>
       </c>
@@ -1411,7 +1408,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="5">
-        <v>43554</v>
+        <v>43769</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -1449,9 +1446,9 @@
       <selection activeCell="B9" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -1459,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -1467,7 +1464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -1475,7 +1472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -1483,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -1499,7 +1496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -1515,7 +1512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>9</v>
       </c>

</xml_diff>